<commit_message>
Add matt g to profiles
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D3921E-3545-4ACB-8C26-7D1C6F62BA92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F095C4-5799-42CF-BC19-3DEF265A3C88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28875" yWindow="-16440" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="138">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Scrum</t>
   </si>
   <si>
-    <t>Adam Cogan is the Chief Architect at SSW, a Microsoft Certified Gold Partner specializing in custom Azure, Azure DevOps (was TFS), .NET, SharePoint and Business Intelligence solutions.​ At SSW, Adam has been developing custom solutions for businesses across a range of industries such as Government, engineering, banking, insurance, and manufacturing since 1990 for clients such as Microsoft, Worley Parsons, and Aurecon. Adam is a Certified Scrum Trainer with scrum.org, trains developers in Australia, the US, UK and Europe, and contributes to scrum.org thinking. He consults with development teams on improving their scrum process through mentoring and being a proxy scrum master. He has written many rules around scrum best practices. Adam is one of only three Microsoft Regional Directors in Australia. In this role, he regularly presents at conferences such as TechEd (USA, Australia, New Zealand, Europe and Malaysia).</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -99,10 +96,6 @@
     <t>.NET MVC</t>
   </si>
   <si>
-    <t>Alex is a .NET Developer with over 5 years of experience consulting on a variety of companies that specialized in Financial Technology, Market Research, Logistics, Construction and Real-Estate to name a few. Always interested in an opportunity to hone his skills, Alex is always up to try new and exciting technologies and challenges to be on the cutting edge, and to help others along the way.​
-​Alex has worked from single-person start-ups to leading a team of developers in building new and exciting products for clients in industries of different forms. ​His main focus is to make sure the team is equipPed for the task and that the clients are involved in being part of the solution building process.</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -118,9 +111,6 @@
     <t>Angular</t>
   </si>
   <si>
-    <t>Alvin Shen is the CEO of SSW China managing SSW Beijing and SSW Hangzhou Office. Alvin has been working in the development realm for more than 13 years, both in China as well as in Australia. In that time, he has established himself as a passionate expert and industry leader. He started as a .NET and SharePoint developer, but through his passion for Scrum and his entrepreneurial spirit, he was able to leverage his skills to become a great Product Owner, as well as a business development manager, and even a CEO of a start-up with 70 people before joining SSW.</t>
-  </si>
-  <si>
     <t>Andreas Lengkeek</t>
   </si>
   <si>
@@ -128,10 +118,6 @@
   </si>
   <si>
     <t>Tennis</t>
-  </si>
-  <si>
-    <t>Andreas is an experienced Software Developer with a demonstrated history of working in the information technology ​​​​and services industry.​ 
-Andreas' main skills​​ focus on .NET Core​, Angular and React applications with bootstrap/material d​esign, leveraging technologies like EF Core and Identity to provide the clients with rich user experiences. Andreas is also passionate about Tennis, playing since he was 10. He likes it so much that he used to take the train by himself after school to head to the practice courts.</t>
   </si>
   <si>
     <t>Andrew Forsyth</t>
@@ -397,9 +383,6 @@
   </si>
   <si>
     <t>Sebastien is a Software Architect with more than 10 years of experience in software development in France, China and now Australia. Before working for SSW, Sebastien worked for the world leading company for HR and Payroll, ADP, for 10 years, developing solutions used to pay hundreds of thousands employees. First using Java/J2EE and Oracle database then .Net/.Net Core, Angular and SQL Server.</t>
-  </si>
-  <si>
-    <t>Toby Goodman</t>
   </si>
   <si>
     <t>Ulysses Maclaren</t>
@@ -448,7 +431,35 @@
     <t>Brendan Richards</t>
   </si>
   <si>
-    <t>Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years. Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. This gives Brendan some unique perspectives on how different teams &amp; platforms have tackled similar problems. Brendan is also one of our training mentors, and he will be presenting here at NDC.</t>
+    <t>Adam Cogan is the Chief Architect at SSW, a Microsoft Certified Gold Partner specializing in custom Azure, Azure DevOps (was TFS), .NET, SharePoint and Business Intelligence solutions.​ At SSW, Adam has been developing custom solutions for businesses across a range of industries including Government, engineering, banking, insurance, and manufacturing since 1990. His clients have included Microsoft, Worley Parsons, and Aurecon. 
+Adam is a Certified Scrum Trainer with scrum.org, trains developers in Australia, the US, UK and Europe, and contributes to scrum.org thinking. He consults with development teams on improving their scrum process through mentoring and being a proxy scrum master and he has written many rules around scrum best practices. 
+Adam is one of only three Microsoft Regional Directors in Australia. In this role, he regularly presents at conferences such as TechEd (USA, Australia, New Zealand, Europe and Malaysia).</t>
+  </si>
+  <si>
+    <t>Alex is a .NET Developer with over 5 years of experience consulting with a variety of companies in fields as diverse as Financial Technology, Market Research, Logistics, Construction and Real-Estate. His diverse experience with these companies goes all the way from single-person start-ups to leading a team of developers in building new and exciting products. 
+Now working as a Software Architect at SSW, Alex is always up for trying new and exciting technologies and facing challenges to hone his skills and remain on the cutting edge. 
+At the same time, he likes to help others along the way – his main focus is to make sure the team is equipped for the task and that his clients are involved in being part of the solution-building process.</t>
+  </si>
+  <si>
+    <t>Alvin Shen is the CEO of SSW China, managing the SSW offices in Beijing and Hangzhou. Alvin has been working in the development realm for more than 13 years, both in China as well as in Australia. In that time, he has established himself as a passionate expert and industry leader. 
+Alvin started as a .NET and SharePoint developer, but through his passion for Scrum and his entrepreneurial spirit, he was able to leverage his skills to become a great Product Owner and business development manager. Prior to joining SSW, Alvin was also CEO of a start-up with 70 people.</t>
+  </si>
+  <si>
+    <t>Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years.  Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. This gives Brendan some unique perspectives on how different teams &amp; platforms have tackled similar problems. Brendan is also one of our training mentors, and he will be presenting here at NDC.</t>
+  </si>
+  <si>
+    <t>Andreas is an experienced Software Developer with a demonstrated history of working in the information technology ​​​​and services industry.​ 
+Andreas' main skills​​ focus on .NET Core​, Angular and React applications with bootstrap/material d​esign, leveraging technologies like EF Core and Identity to provide the clients with rich user experiences. Andreas is also passionate about Tennis, playing since he was 10. He likes it so much that he used to take the train by himself after school to head to the practice courts.</t>
+  </si>
+  <si>
+    <t>Matt Goldman</t>
+  </si>
+  <si>
+    <t>Xamarin</t>
+  </si>
+  <si>
+    <t>Matt has worked in IT for 15 years, with a background in infrastructure and management, and has delivered security policies, IT strategies and disaster recovery plans to a number of high profile national and multi-national clients.
+Drawing on a combination of hands-on experience and enterprise governance practices, Matt is able to make connections between business and technology to deliver user and business focused outcomes.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -539,30 +550,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -572,30 +559,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -615,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -627,9 +590,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -659,34 +619,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1005,1064 +941,1076 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.15234375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="17.53515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="64.3828125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="28.53515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="15.15234375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="13.53515625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="17.53515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.53515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.53515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" style="7" customWidth="1"/>
     <col min="12" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="221.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="189.45" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="131.15" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="140.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="131.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>32</v>
+      <c r="C5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="H5" s="3">
         <v>165</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>16</v>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="H6" s="3">
         <v>225</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="134.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="14">
         <v>245</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="134.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="3"/>
+      <c r="I7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="106.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="22" t="s">
+      <c r="G9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="H9" s="15">
+        <v>245</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="131.15" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="F10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="24">
-        <v>245</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="155.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H10" s="3">
         <v>165</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>55</v>
+      <c r="F11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H11" s="3">
         <v>245</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="G12" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="H12" s="3">
         <v>245</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="169.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="H13" s="3">
         <v>205</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="14"/>
+        <v>65</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="13"/>
       <c r="G14" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H14" s="3">
         <v>285</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="108" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="H15" s="3">
         <v>285</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="H16" s="3">
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="124" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
       <c r="G17" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H17" s="3">
         <v>245</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="H18" s="3">
         <v>50</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>87</v>
+        <v>35</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H19" s="3">
         <v>245</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>90</v>
+        <v>65</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>94</v>
+      <c r="E21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H21" s="3">
         <v>285</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="116.15" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>99</v>
+        <v>17</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="102.65" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="14"/>
+      <c r="E23" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="G23" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H23" s="3">
         <v>225</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="126.65" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="C24" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H24" s="3">
         <v>285</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="176.15" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="14"/>
+      <c r="E25" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="13"/>
       <c r="G25" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H25" s="3">
         <v>245</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>90</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H26" s="3">
         <v>245</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="162.65" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>116</v>
+        <v>35</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="161.15" customHeight="1" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="14"/>
+        <v>110</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>112</v>
+      </c>
       <c r="G28" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H28" s="3">
         <v>205</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="H29" s="3">
         <v>50</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="14"/>
+      <c r="E30" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="13"/>
       <c r="G30" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H30" s="3">
         <v>225</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="158.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="H31" s="3">
         <v>285</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2086,6 +2034,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2243,12 +2197,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
@@ -2258,6 +2206,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2273,20 +2237,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix liam elliott name
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F095C4-5799-42CF-BC19-3DEF265A3C88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CB5B41-5E84-4079-A94B-F972ADA31266}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28875" yWindow="-16440" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,9 +290,6 @@
 Kosta’s experience covers developing software using several programming languages and technologies, practical data analysis, designing and developing solutions from scratch as well as promptly improving, debugging and optimising clients’ systems. SSW is a Zendesk Partner and Kosta is one of our Zendesk experts.</t>
   </si>
   <si>
-    <t>Liam Elliot</t>
-  </si>
-  <si>
     <t>Running</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   <si>
     <t>Matt has worked in IT for 15 years, with a background in infrastructure and management, and has delivered security policies, IT strategies and disaster recovery plans to a number of high profile national and multi-national clients.
 Drawing on a combination of hands-on experience and enterprise governance practices, Matt is able to make connections between business and technology to deliver user and business focused outcomes.</t>
+  </si>
+  <si>
+    <t>Liam Elliott</t>
   </si>
 </sst>
 </file>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1009,7 +1009,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
@@ -1074,10 +1074,10 @@
         <v>25</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
@@ -1112,7 +1112,7 @@
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" s="3">
         <v>165</v>
@@ -1135,13 +1135,13 @@
         <v>30</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>32</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="8" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>65</v>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>65</v>
@@ -1624,10 +1624,10 @@
         <v>25</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="21" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>13</v>
@@ -1659,10 +1659,10 @@
         <v>24</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="H21" s="3">
         <v>285</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="22" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
@@ -1691,13 +1691,13 @@
         <v>25</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="23" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>39</v>
@@ -1726,13 +1726,13 @@
         <v>14</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="G23" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="H23" s="3">
         <v>225</v>
@@ -1749,10 +1749,10 @@
     </row>
     <row r="24" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>39</v>
@@ -1761,11 +1761,11 @@
         <v>14</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H24" s="3">
         <v>285</v>
@@ -1780,23 +1780,23 @@
     </row>
     <row r="25" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="3">
         <v>245</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="26" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" s="3">
         <v>245</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="27" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
@@ -1856,13 +1856,13 @@
         <v>18</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
@@ -1879,25 +1879,25 @@
     </row>
     <row r="28" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F28" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="H28" s="3">
         <v>205</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="29" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -1926,11 +1926,11 @@
         <v>18</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H29" s="3">
         <v>50</v>
@@ -1947,23 +1947,23 @@
     </row>
     <row r="30" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="C30" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H30" s="3">
         <v>225</v>
@@ -1980,25 +1980,25 @@
     </row>
     <row r="31" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="E31" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="F31" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="G31" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="H31" s="3">
         <v>285</v>
@@ -2025,21 +2025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2197,10 +2182,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2222,19 +2232,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added twitter usernames to data seeding
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\src\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CB5B41-5E84-4079-A94B-F972ADA31266}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE0B682-6557-4CFD-991A-0DB43CA20351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28875" yWindow="-16440" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$31</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="151">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -460,6 +460,45 @@
   </si>
   <si>
     <t>Liam Elliott</t>
+  </si>
+  <si>
+    <t>Twitter Username</t>
+  </si>
+  <si>
+    <t>adamcogan</t>
+  </si>
+  <si>
+    <t>GregHarrisSSW</t>
+  </si>
+  <si>
+    <t>Jean_SSW</t>
+  </si>
+  <si>
+    <t>jernej_kavka</t>
+  </si>
+  <si>
+    <t>madkonst</t>
+  </si>
+  <si>
+    <t>liamelliott_au</t>
+  </si>
+  <si>
+    <t>matteightyate</t>
+  </si>
+  <si>
+    <t>MattGoldmanSSW</t>
+  </si>
+  <si>
+    <t>michaelsmedley</t>
+  </si>
+  <si>
+    <t>PennyWalker_SSW</t>
+  </si>
+  <si>
+    <t>ulyssesmac</t>
+  </si>
+  <si>
+    <t>William_DotNet</t>
   </si>
 </sst>
 </file>
@@ -939,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -951,14 +990,14 @@
     <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="17.53515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.53515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.53515625" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.84375" style="2"/>
+    <col min="8" max="9" width="28.53515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.53515625" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -984,16 +1023,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="247.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1057,7 @@
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>15</v>
@@ -1023,8 +1065,11 @@
       <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="189.45" x14ac:dyDescent="0.4">
+      <c r="L2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1047,17 +1092,18 @@
       <c r="H3" s="3">
         <v>205</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="131.15" x14ac:dyDescent="0.4">
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1082,17 +1128,18 @@
       <c r="H4" s="3">
         <v>225</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="L4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1117,17 +1164,18 @@
       <c r="H5" s="3">
         <v>165</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="L5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1152,17 +1200,18 @@
       <c r="H6" s="3">
         <v>225</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="L6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1187,17 +1236,18 @@
       <c r="H7" s="14">
         <v>245</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>21</v>
-      </c>
+      <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="L7" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>128</v>
       </c>
@@ -1220,17 +1270,18 @@
       <c r="H8" s="3">
         <v>245</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1255,17 +1306,18 @@
       <c r="H9" s="15">
         <v>245</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="I9" s="15"/>
       <c r="J9" s="15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K9" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="131.15" x14ac:dyDescent="0.4">
+      <c r="L9" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1290,17 +1342,18 @@
       <c r="H10" s="3">
         <v>165</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -1325,17 +1378,18 @@
       <c r="H11" s="3">
         <v>245</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1361,16 +1415,19 @@
         <v>245</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="L12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -1393,17 +1450,18 @@
       <c r="H13" s="3">
         <v>205</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
@@ -1426,17 +1484,18 @@
       <c r="H14" s="3">
         <v>285</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -1462,7 +1521,7 @@
         <v>285</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>15</v>
@@ -1470,8 +1529,11 @@
       <c r="K15" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -1497,16 +1559,19 @@
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+      <c r="L16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -1529,17 +1594,18 @@
       <c r="H17" s="3">
         <v>245</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>77</v>
       </c>
@@ -1562,17 +1628,18 @@
       <c r="H18" s="3">
         <v>50</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -1598,7 +1665,7 @@
         <v>245</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>21</v>
@@ -1606,8 +1673,11 @@
       <c r="K19" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+      <c r="L19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>137</v>
       </c>
@@ -1633,16 +1703,19 @@
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -1668,7 +1741,7 @@
         <v>285</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>15</v>
@@ -1676,8 +1749,11 @@
       <c r="K21" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="L21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>134</v>
       </c>
@@ -1703,16 +1779,19 @@
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -1737,17 +1816,18 @@
       <c r="H23" s="3">
         <v>225</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -1770,15 +1850,18 @@
       <c r="H24" s="3">
         <v>285</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I24" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+      <c r="L24" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -1801,17 +1884,18 @@
       <c r="H25" s="3">
         <v>245</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I25" s="3"/>
       <c r="J25" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
@@ -1835,14 +1919,15 @@
         <v>245</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="J26" s="3"/>
       <c r="K26" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L26" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
@@ -1867,17 +1952,18 @@
       <c r="H27" s="3">
         <v>225</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I27" s="3"/>
       <c r="J27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="L27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>108</v>
       </c>
@@ -1903,7 +1989,7 @@
         <v>205</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>21</v>
+        <v>148</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>21</v>
@@ -1911,8 +1997,11 @@
       <c r="K28" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="L28" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1935,17 +2024,18 @@
       <c r="H29" s="3">
         <v>50</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="L29" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1969,16 +2059,19 @@
         <v>225</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="145.75" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
@@ -2004,7 +2097,7 @@
         <v>285</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>21</v>
@@ -2012,10 +2105,13 @@
       <c r="K31" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="L31" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K31" xr:uid="{9AA24026-1D6B-4950-9702-5DBD73A8EC72}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
+  <autoFilter ref="A1:L31" xr:uid="{9AA24026-1D6B-4950-9702-5DBD73A8EC72}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L31">
       <sortCondition ref="A1:A31"/>
     </sortState>
   </autoFilter>
@@ -2025,6 +2121,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2182,35 +2293,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2232,9 +2318,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cut some profiles to fit
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA0AAF-8939-47F9-A919-35E5A3118D15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D072DA92-6DEF-4E76-9A92-CD98326E0CFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="155">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Planting roses</t>
   </si>
   <si>
-    <t>Anthony is a Senior Software Architect in the Brisbane office and brings 20 years of development experience across many industries including stockbroking, microfinance and point of sale. He has a keen interest in software and database performance, reducing running costs and reducing problems through simple solutions. His experience in team lead and agile coaching roles contributes to his ability to produce great outcomes for clients. He would escape to a hobby farm in the country, given half a chance, even though his horticultural skills leave much to be desired.</t>
-  </si>
-  <si>
     <t>Calum Simpson</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>Singer</t>
   </si>
   <si>
-    <t>​Chris is a professional software developer specialising in web-development, following new mobile and web technologies around the world.​ He is an Angular and .NET Core specialist, supported by his experiences in many technologies, which includes: C#, HTML, CSS, Javascript, Java/Kotlin, SQL, Python, and Android. Additionally, Chris is also experienced in embedded devices - particularly real-time systems and IoT devices using various hardware such as Raspberry Pi​, ESP8266, and others​. When not in work mode, Chris have as a hobby nature photography, and he actively participates as a singer in his youth community choir.</t>
-  </si>
-  <si>
     <t>Gabriel George</t>
   </si>
   <si>
@@ -222,10 +216,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>​​​​​​​​​​​​​​Jack is a motivated IT and Business graduate with a wealth of experience developing​ native mobile applications and web apps. Jack has been involved in projects for a variety of organisations ranging from small technology start-up​​s​ to large TNC's. His work has enabled him to develop multiple mobile and web applications and be instrumental in the orchestration of large digital transformation projects.
-His areas of interest include machine learning, mobile application development, embedded systems​ development, user interaction design and artificial intelligence.​</t>
-  </si>
-  <si>
     <t>Jason Taylor</t>
   </si>
   <si>
@@ -257,9 +247,6 @@
   </si>
   <si>
     <t>Jerry Luo</t>
-  </si>
-  <si>
-    <t>​​With 10 years working experience in software industry, Jerry is a developer, technical lead, and software architect. All round developer who is good at software architecture and back-end API development. Jerry has worked for several different types of IT companies. He has experience in many challenging projects like Knowledge Sharing, IM, Logistics Supply Chain. Jerry likes learning new technologies and helping business to successfully achieve their goals through tech. ​</t>
   </si>
   <si>
     <t>Ken Shi</t>
@@ -317,9 +304,6 @@
     <t>Baseball</t>
   </si>
   <si>
-    <t>Matthew is the SSW Manager of Queensland and International clients. Operating from the SSW office in Brisbane CBD, Matthew is in charge of looking after SSW's global clients in Europe, Asia, Africa, and beyond. Matthew has over 10 years of experience as a technology consultant and team leader, having worked in both capacities for businesses such as DXC and Accenture. Originally from the US, Matthew is an avid fan of MLB baseball and NFL football.</t>
-  </si>
-  <si>
     <t>Michael Smedley</t>
   </si>
   <si>
@@ -344,10 +328,6 @@
     <t>Patrick Zhao</t>
   </si>
   <si>
-    <t xml:space="preserve">​​​Patrick is a passionate full stack software engineer with more than 5 years of professional experience in FinTech industry. Patrick joined SSW as a Senior Software Architect with focus on building enterprise web applications utilizing modern technologies such as ASP.NET Core, EF Core, Angular, SignalR, SQL, Machine Learning and Azure DevOps.
-Patrick has recently been focusing on IoT, serverless applications and machine learning. ​Patrick is a motivated software engineer, scrum practitioner and outstanding team player. Patrick is good at taking the initiative, conducting research and proposing solutions for different business requirements. </t>
-  </si>
-  <si>
     <t>Patricia Barros</t>
   </si>
   <si>
@@ -369,10 +349,6 @@
     <t>Dragonboating</t>
   </si>
   <si>
-    <t>Thanks to Penny's positive energy and strong people skills she is the face of SSW recruitment. She seeks the best people to expand our awesome SSW family, and then helps them settle in with a unique, personal​​ on-boarding experience. ​​​​
-​​​​​​​​​Penny is usually described as SSW's "Chief Problem Solver" (that's what you'll see on her signature), but in reality she works across a few different teams. She's an Account Manager, Marketing Officer and Administrator. She is also the go-to person if you ever need help, or if you have a problem that you cannot solve. Besides (all of) that, she's also a museum nerd, football coach and loves dragonboating!</t>
-  </si>
-  <si>
     <t>Sébastien Boissière</t>
   </si>
   <si>
@@ -388,11 +364,6 @@
     <t>Salsa</t>
   </si>
   <si>
-    <t>Scrum Master for internal development teams, the design, video, and marketing teams, as well as client projects. Integrity, transparency, and a smooth running team are all very important to him. He's also a Power BI guru. _x000D_
-_x000D_
-In his spare time, he is one of Australia's top Salsa teachers and is the 5 times Australian Salsa Champion, 5 times Australian Bachata Champion, and part of the Bachata World Champion team</t>
-  </si>
-  <si>
     <t>William Liebenberg</t>
   </si>
   <si>
@@ -408,11 +379,6 @@
     <t>Presenting talks</t>
   </si>
   <si>
-    <t xml:space="preserve">William is a Solution Architect at SSW Melbourne with a strong focus on Azure, Automation, DevOps, and Serverless. He works closely with clients to build solutions, mentor development teams and having fun during the whole process.
-In his spare time, he dives into the world of Bots, Machine Learning and 3D Graphics... then go on tropical holidays!
-William is an active member of the Melbourne developer community where you can find him attending or presenting at user groups, hack days and conferences every time he has a chance! He is a mentor on the Azure Superpowers tour and also President of the Melbourne .NET User Group. </t>
-  </si>
-  <si>
     <t>Scuba diving</t>
   </si>
   <si>
@@ -423,22 +389,6 @@
   </si>
   <si>
     <t>Brendan Richards</t>
-  </si>
-  <si>
-    <t>Alex is a .NET Developer with over 5 years of experience consulting with a variety of companies in fields as diverse as Financial Technology, Market Research, Logistics, Construction and Real-Estate. His diverse experience with these companies goes all the way from single-person start-ups to leading a team of developers in building new and exciting products. 
-Now working as a Software Architect at SSW, Alex is always up for trying new and exciting technologies and facing challenges to hone his skills and remain on the cutting edge. 
-At the same time, he likes to help others along the way – his main focus is to make sure the team is equipped for the task and that his clients are involved in being part of the solution-building process.</t>
-  </si>
-  <si>
-    <t>Alvin Shen is the CEO of SSW China, managing the SSW offices in Beijing and Hangzhou. Alvin has been working in the development realm for more than 13 years, both in China as well as in Australia. In that time, he has established himself as a passionate expert and industry leader. 
-Alvin started as a .NET and SharePoint developer, but through his passion for Scrum and his entrepreneurial spirit, he was able to leverage his skills to become a great Product Owner and business development manager. Prior to joining SSW, Alvin was also CEO of a start-up with 70 people.</t>
-  </si>
-  <si>
-    <t>Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years.  Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. This gives Brendan some unique perspectives on how different teams &amp; platforms have tackled similar problems. Brendan is also one of our training mentors, and he will be presenting here at NDC.</t>
-  </si>
-  <si>
-    <t>Andreas is an experienced Software Developer with a demonstrated history of working in the information technology ​​​​and services industry.​ 
-Andreas' main skills​​ focus on .NET Core​, Angular and React applications with bootstrap/material d​esign, leveraging technologies like EF Core and Identity to provide the clients with rich user experiences. Andreas is also passionate about Tennis, playing since he was 10. He likes it so much that he used to take the train by himself after school to head to the practice courts.</t>
   </si>
   <si>
     <t>Matt Goldman</t>
@@ -490,12 +440,69 @@
     <t>William_DotNet</t>
   </si>
   <si>
-    <t>Adam Cogan is the Chief Architect at SSW, a Microsoft Certified Gold Partner specializing in Azure, Azure DevOps, .NET, SharePoint and BI solutions.​ At SSW, Adam has been developing custom solutions for businesses across a range of industries including Government, engineering, banking, insurance, and manufacturing since 1990.
-Adam is a Certified Scrum Trainer with scrum.org, trains developers in Australia, the US, UK and Europe, and contributes to scrum.org thinking. He consults with development teams on improving their scrum process through mentoring and being a proxy scrum master.
-As one of only three Microsoft Regional Directors in Australia, he regularly presents at international conferences.</t>
-  </si>
-  <si>
     <t>MattGoldman</t>
+  </si>
+  <si>
+    <t>Adam Cogan is the Chief Architect at SSW, a Microsoft Certified Gold Partner specializing in Azure, Azure DevOps, .NET, SharePoint and BI solutions.​ At SSW, Adam has been developing custom solutions for businesses across a range of industries including Government, engineering, banking, insurance, and manufacturing since 1990.</t>
+  </si>
+  <si>
+    <t>AndreasLengkeek</t>
+  </si>
+  <si>
+    <t>isonaj</t>
+  </si>
+  <si>
+    <t>brendanssw</t>
+  </si>
+  <si>
+    <t>geo_ge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex is a .NET Developer with over 5 years of experience consulting with a variety of companies in fields as diverse as Financial Technology, Market Research, Logistics, Construction and Real-Estate. His diverse experience with these companies goes all the way from single-person start-ups to leading a team of developers in building new and exciting products. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alvin Shen is the CEO of SSW China, managing the SSW offices in Beijing and Hangzhou. Alvin has been working in the development realm for more than 13 years, both in China as well as in Australia. In that time, he has established himself as a passionate expert and industry leader. </t>
+  </si>
+  <si>
+    <t>Andreas is an experienced Software Developer with a demonstrated history of working in the information technology ​​​​and services industry.​ 
+Andreas' main skills​​ focus on .NET Core​, Angular and React applications with bootstrap/material d​esign, leveraging technologies like EF Core and Identity to provide the clients with rich user experiences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthony is a Senior Software Architect in the Brisbane office and brings 20 years of development experience across many industries including stockbroking, microfinance and point of sale. He has a keen interest in software and database performance, reducing running costs and reducing problems through simple solutions. His experience in team lead and agile coaching roles contributes to his ability to produce great outcomes for clients. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years.  Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. </t>
+  </si>
+  <si>
+    <t>​Chris is a professional software developer specialising in web-development, following new mobile and web technologies around the world.​ He is an Angular and .NET Core specialist, supported by his experiences in many technologies, which includes: C#, HTML, CSS, Javascript, Java/Kotlin, SQL, Python, and Android. Additionally, Chris is also experienced in embedded devices - particularly real-time systems and IoT devices using various hardware such as Raspberry Pi​, ESP8266, and others​.</t>
+  </si>
+  <si>
+    <t>talentJ</t>
+  </si>
+  <si>
+    <t>​​​​​​​​​​​​​​Jack is a motivated IT and Business graduate with a wealth of experience developing​ native mobile applications and web apps. Jack has been involved in projects for a variety of organisations ranging from small technology start-up​​s​ to large TNC's. His work has enabled him to develop multiple mobile and web applications and be instrumental in the orchestration of large digital transformation projects.</t>
+  </si>
+  <si>
+    <t>​​With 10 years working experience in software industry, Jerry is a developer, technical lead, and software architect. All round developer who is good at software architecture and back-end API development. Jerry has worked for several different types of IT companies. He has experience in many challenging projects like Knowledge Sharing, IM, Logistics Supply Chain.</t>
+  </si>
+  <si>
+    <t>Matthew is the SSW Manager of Queensland and International clients. Operating from the SSW office in Brisbane CBD, Matthew is in charge of looking after SSW's global clients in Europe, Asia, Africa, and beyond. Matthew has over 10 years of experience as a technology consultant and team leader, having worked in both capacities for businesses such as DXC and Accenture.</t>
+  </si>
+  <si>
+    <t>​​​Patrick is a passionate full stack software engineer with more than 5 years of professional experience in FinTech industry. Patrick joined SSW as a Senior Software Architect with focus on building enterprise web applications utilizing modern technologies such as ASP.NET Core, EF Core, Angular, SignalR, SQL, Machine Learning and Azure DevOps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks to Penny's positive energy and strong people skills she is the face of SSW recruitment. She seeks the best people to expand our awesome SSW family, and then helps them settle in with a unique, personal​​ on-boarding experience. ​​​​
+​​​​​​​​​Penny is usually described as SSW's "Chief Problem Solver" (that's what you'll see on her signature), but in reality she works across a few different teams. </t>
+  </si>
+  <si>
+    <t>Scrum Master for internal development teams, the design, video, and marketing teams, as well as client projects. Integrity, transparency, and a smooth running team are all very important to him. He's also a Power BI guru. 
+In his spare time, he is one of Australia's top Salsa teachers and is the 5 times Australian Salsa Champion, 5 times Australian Bachata Champion, and part of the Bachata World Champion team</t>
+  </si>
+  <si>
+    <t>William is a Solution Architect at SSW Melbourne with a strong focus on Azure, Automation, DevOps, and Serverless. He works closely with clients to build solutions, mentor development teams and having fun during the whole process.
+In his spare time, he dives into the world of Bots, Machine Learning and 3D Graphics... then go on tropical holidays!</t>
   </si>
 </sst>
 </file>
@@ -977,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1020,7 +1027,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>8</v>
@@ -1032,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="189.45" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1048,13 +1055,13 @@
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>15</v>
@@ -1066,7 +1073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="189.45" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1091,7 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
@@ -1100,7 +1107,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="131.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1117,10 +1124,10 @@
         <v>25</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
@@ -1136,7 +1143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1156,12 +1163,14 @@
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="H5" s="3">
         <v>165</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
@@ -1180,13 +1189,13 @@
         <v>30</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>32</v>
@@ -1208,7 +1217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1228,12 +1237,14 @@
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="H7" s="14">
         <v>245</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="J7" s="14" t="s">
         <v>21</v>
       </c>
@@ -1244,12 +1255,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>18</v>
@@ -1258,16 +1269,18 @@
         <v>24</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1280,25 +1293,25 @@
     </row>
     <row r="9" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="H9" s="15">
         <v>245</v>
@@ -1314,12 +1327,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>25</v>
@@ -1328,13 +1341,13 @@
         <v>18</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="H10" s="3">
         <v>165</v>
@@ -1352,7 +1365,7 @@
     </row>
     <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>35</v>
@@ -1361,21 +1374,23 @@
         <v>25</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H11" s="3">
         <v>245</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="J11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1388,31 +1403,31 @@
     </row>
     <row r="12" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G12" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="H12" s="3">
         <v>245</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>21</v>
@@ -1424,25 +1439,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="3" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="H13" s="3">
         <v>205</v>
@@ -1460,10 +1475,10 @@
     </row>
     <row r="14" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>18</v>
@@ -1476,7 +1491,7 @@
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3">
         <v>285</v>
@@ -1494,31 +1509,31 @@
     </row>
     <row r="15" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H15" s="3">
         <v>285</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>15</v>
@@ -1532,7 +1547,7 @@
     </row>
     <row r="16" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>35</v>
@@ -1541,20 +1556,20 @@
         <v>18</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H16" s="3">
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>21</v>
@@ -1566,9 +1581,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
@@ -1577,14 +1592,14 @@
         <v>18</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="3" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="H17" s="3">
         <v>245</v>
@@ -1602,28 +1617,30 @@
     </row>
     <row r="18" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H18" s="3">
         <v>50</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="J18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1636,7 +1653,7 @@
     </row>
     <row r="19" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>35</v>
@@ -1651,16 +1668,16 @@
         <v>20</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H19" s="3">
         <v>245</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>21</v>
@@ -1674,31 +1691,31 @@
     </row>
     <row r="20" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>21</v>
@@ -1712,13 +1729,13 @@
     </row>
     <row r="21" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>13</v>
@@ -1727,16 +1744,16 @@
         <v>24</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H21" s="3">
         <v>285</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>15</v>
@@ -1750,7 +1767,7 @@
     </row>
     <row r="22" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
@@ -1762,19 +1779,19 @@
         <v>25</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>21</v>
@@ -1786,27 +1803,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>94</v>
+        <v>150</v>
       </c>
       <c r="H23" s="3">
         <v>225</v>
@@ -1824,29 +1841,29 @@
     </row>
     <row r="24" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H24" s="3">
         <v>285</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
@@ -1858,23 +1875,23 @@
     </row>
     <row r="25" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H25" s="3">
         <v>245</v>
@@ -1890,9 +1907,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -1908,7 +1925,7 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="H26" s="3">
         <v>245</v>
@@ -1924,7 +1941,7 @@
     </row>
     <row r="27" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
@@ -1936,13 +1953,13 @@
         <v>18</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
@@ -1958,33 +1975,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="H28" s="3">
         <v>205</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>21</v>
@@ -1998,7 +2015,7 @@
     </row>
     <row r="29" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -2010,11 +2027,11 @@
         <v>18</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H29" s="3">
         <v>50</v>
@@ -2032,29 +2049,29 @@
     </row>
     <row r="30" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="3" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="H30" s="3">
         <v>225</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>15</v>
@@ -2066,33 +2083,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="H31" s="3">
         <v>285</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>21</v>
@@ -2116,6 +2133,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2273,35 +2305,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2323,9 +2330,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add more profile images
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D072DA92-6DEF-4E76-9A92-CD98326E0CFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1A103-A37F-4A12-A26B-BFB99F1564CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="160">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -243,9 +243,6 @@
     <t>ML.NET</t>
   </si>
   <si>
-    <t>JK is SSW’s Mr AI. While he has 10 years of experience in software engineering building web applications across multiple industries around the world, his latest passion lies in AI, Cognitive Services and Facial Recognition which he used to build SSW Sophie AI. Most recently, JK has been presenting at cool tech conferences all around Australia, including here at NDC. He's also a Wisecrack addict.</t>
-  </si>
-  <si>
     <t>Jerry Luo</t>
   </si>
   <si>
@@ -261,23 +258,13 @@
     <t>Photoshop</t>
   </si>
   <si>
-    <t>Ken is a Product Designer at SSW Hangzhou Office. He has been working in the interactive design industry for more than 10 years, both in China and Australia. After graduating from the University of Queensland, he co-founded 2 start-ups over 7 years before joining SSW in 2019. At SSW he has been focusing on media and creation experiences, working on SSW products like SugarLearning.</t>
-  </si>
-  <si>
     <t>Kosta Madorski</t>
   </si>
   <si>
     <t>Rock Climbing</t>
   </si>
   <si>
-    <t>Kosta is a Senior Software Architect based in SSW's Sydney office. He is passionate about innovations and effective delivery of services.
-Kosta’s experience covers developing software using several programming languages and technologies, practical data analysis, designing and developing solutions from scratch as well as promptly improving, debugging and optimising clients’ systems. SSW is a Zendesk Partner and Kosta is one of our Zendesk experts.</t>
-  </si>
-  <si>
     <t>Running</t>
-  </si>
-  <si>
-    <t>Liam has been a software developer for over 12 years and he is also a certified Scrum Master. His experience is vast, having worked across a number of industries, like telecommunication, foreign exchange, legal, HR sectors &amp; more. Liam's current projects include technologies like ASP.NET Core Web API's with Angular 8, and React front-ends. Liam shares his passion and experience for modern technologies through user groups, and training events.</t>
   </si>
   <si>
     <t>Matt Wicks</t>
@@ -465,44 +452,72 @@
     <t xml:space="preserve">Alvin Shen is the CEO of SSW China, managing the SSW offices in Beijing and Hangzhou. Alvin has been working in the development realm for more than 13 years, both in China as well as in Australia. In that time, he has established himself as a passionate expert and industry leader. </t>
   </si>
   <si>
+    <t xml:space="preserve">Anthony is a Senior Software Architect in the Brisbane office and brings 20 years of development experience across many industries including stockbroking, microfinance and point of sale. He has a keen interest in software and database performance, reducing running costs and reducing problems through simple solutions. His experience in team lead and agile coaching roles contributes to his ability to produce great outcomes for clients. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years.  Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. </t>
+  </si>
+  <si>
+    <t>​Chris is a professional software developer specialising in web-development, following new mobile and web technologies around the world.​ He is an Angular and .NET Core specialist, supported by his experiences in many technologies, which includes: C#, HTML, CSS, Javascript, Java/Kotlin, SQL, Python, and Android. Additionally, Chris is also experienced in embedded devices - particularly real-time systems and IoT devices using various hardware such as Raspberry Pi​, ESP8266, and others​.</t>
+  </si>
+  <si>
+    <t>talentJ</t>
+  </si>
+  <si>
+    <t>​​​​​​​​​​​​​​Jack is a motivated IT and Business graduate with a wealth of experience developing​ native mobile applications and web apps. Jack has been involved in projects for a variety of organisations ranging from small technology start-up​​s​ to large TNC's. His work has enabled him to develop multiple mobile and web applications and be instrumental in the orchestration of large digital transformation projects.</t>
+  </si>
+  <si>
+    <t>Matthew is the SSW Manager of Queensland and International clients. Operating from the SSW office in Brisbane CBD, Matthew is in charge of looking after SSW's global clients in Europe, Asia, Africa, and beyond. Matthew has over 10 years of experience as a technology consultant and team leader, having worked in both capacities for businesses such as DXC and Accenture.</t>
+  </si>
+  <si>
+    <t>​​​Patrick is a passionate full stack software engineer with more than 5 years of professional experience in FinTech industry. Patrick joined SSW as a Senior Software Architect with focus on building enterprise web applications utilizing modern technologies such as ASP.NET Core, EF Core, Angular, SignalR, SQL, Machine Learning and Azure DevOps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks to Penny's positive energy and strong people skills she is the face of SSW recruitment. She seeks the best people to expand our awesome SSW family, and then helps them settle in with a unique, personal​​ on-boarding experience. ​​​​
+​​​​​​​​​Penny is usually described as SSW's "Chief Problem Solver" (that's what you'll see on her signature), but in reality she works across a few different teams. </t>
+  </si>
+  <si>
+    <t>William is a Solution Architect at SSW Melbourne with a strong focus on Azure, Automation, DevOps, and Serverless. He works closely with clients to build solutions, mentor development teams and having fun during the whole process.
+In his spare time, he dives into the world of Bots, Machine Learning and 3D Graphics... then go on tropical holidays!</t>
+  </si>
+  <si>
+    <t>my304</t>
+  </si>
+  <si>
+    <t>JasonGtAu</t>
+  </si>
+  <si>
+    <t>MicrosoftApple</t>
+  </si>
+  <si>
+    <t>patribarros1</t>
+  </si>
+  <si>
+    <t>Liam has been a software developer for over 12 years and he is also a certified Scrum Master. His experience is vast, having worked across a number of industries, like telecommunication, foreign exchange, legal, HR sectors &amp; more. Liam's current projects include technologies like ASP.NET Core Web API's with Angular 8, and React front-ends.</t>
+  </si>
+  <si>
+    <t>Ken is a Product Designer at SSW Hangzhou Office. He has been working in the interactive design industry for more than 10 years, both in China and Australia. After graduating from the University of Queensland, he co-founded 2 start-ups over 7 years before joining SSW in 2019.</t>
+  </si>
+  <si>
+    <t>​​With 10 years working experience in software industry, Jerry is a developer, technical lead, and software architect. All round developer who is good at software architecture and back-end API development. Jerry has worked for several different types of IT companies.</t>
+  </si>
+  <si>
+    <t>JK is SSW’s Mr AI. While he has 10 years of experience in software engineering building web applications across multiple industries around the world, his latest passion lies in AI, Cognitive Services and Facial Recognition which he used to build SSW Sophie AI. Most recently, JK has been presenting at cool tech conferences all around Australia, including here at NDC.</t>
+  </si>
+  <si>
+    <t>Kosta is a Senior Software Architect based in SSW's Sydney office. He is passionate about innovations and effective delivery of services.
+Kosta’s experience covers developing software using several programming languages and technologies, practical data analysis, designing and developing solutions from scratch as well as promptly improving, debugging and optimising clients’ systems.</t>
+  </si>
+  <si>
     <t>Andreas is an experienced Software Developer with a demonstrated history of working in the information technology ​​​​and services industry.​ 
 Andreas' main skills​​ focus on .NET Core​, Angular and React applications with bootstrap/material d​esign, leveraging technologies like EF Core and Identity to provide the clients with rich user experiences.</t>
   </si>
   <si>
-    <t xml:space="preserve">Anthony is a Senior Software Architect in the Brisbane office and brings 20 years of development experience across many industries including stockbroking, microfinance and point of sale. He has a keen interest in software and database performance, reducing running costs and reducing problems through simple solutions. His experience in team lead and agile coaching roles contributes to his ability to produce great outcomes for clients. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Throughout his career, Brendan has been a big user and proponent of Open Source software. This has been applied to a broad variety of web-based programming projects spanning the last 17 years.  Brendan has worked with an eclectic mix of languages, platforms and technologies including .Net, Java, PHP, Ruby and Perl across both Unix/Linux and Microsoft Windows platforms. </t>
-  </si>
-  <si>
-    <t>​Chris is a professional software developer specialising in web-development, following new mobile and web technologies around the world.​ He is an Angular and .NET Core specialist, supported by his experiences in many technologies, which includes: C#, HTML, CSS, Javascript, Java/Kotlin, SQL, Python, and Android. Additionally, Chris is also experienced in embedded devices - particularly real-time systems and IoT devices using various hardware such as Raspberry Pi​, ESP8266, and others​.</t>
-  </si>
-  <si>
-    <t>talentJ</t>
-  </si>
-  <si>
-    <t>​​​​​​​​​​​​​​Jack is a motivated IT and Business graduate with a wealth of experience developing​ native mobile applications and web apps. Jack has been involved in projects for a variety of organisations ranging from small technology start-up​​s​ to large TNC's. His work has enabled him to develop multiple mobile and web applications and be instrumental in the orchestration of large digital transformation projects.</t>
-  </si>
-  <si>
-    <t>​​With 10 years working experience in software industry, Jerry is a developer, technical lead, and software architect. All round developer who is good at software architecture and back-end API development. Jerry has worked for several different types of IT companies. He has experience in many challenging projects like Knowledge Sharing, IM, Logistics Supply Chain.</t>
-  </si>
-  <si>
-    <t>Matthew is the SSW Manager of Queensland and International clients. Operating from the SSW office in Brisbane CBD, Matthew is in charge of looking after SSW's global clients in Europe, Asia, Africa, and beyond. Matthew has over 10 years of experience as a technology consultant and team leader, having worked in both capacities for businesses such as DXC and Accenture.</t>
-  </si>
-  <si>
-    <t>​​​Patrick is a passionate full stack software engineer with more than 5 years of professional experience in FinTech industry. Patrick joined SSW as a Senior Software Architect with focus on building enterprise web applications utilizing modern technologies such as ASP.NET Core, EF Core, Angular, SignalR, SQL, Machine Learning and Azure DevOps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanks to Penny's positive energy and strong people skills she is the face of SSW recruitment. She seeks the best people to expand our awesome SSW family, and then helps them settle in with a unique, personal​​ on-boarding experience. ​​​​
-​​​​​​​​​Penny is usually described as SSW's "Chief Problem Solver" (that's what you'll see on her signature), but in reality she works across a few different teams. </t>
+    <t>mozdemir_au</t>
   </si>
   <si>
     <t>Scrum Master for internal development teams, the design, video, and marketing teams, as well as client projects. Integrity, transparency, and a smooth running team are all very important to him. He's also a Power BI guru. 
-In his spare time, he is one of Australia's top Salsa teachers and is the 5 times Australian Salsa Champion, 5 times Australian Bachata Champion, and part of the Bachata World Champion team</t>
-  </si>
-  <si>
-    <t>William is a Solution Architect at SSW Melbourne with a strong focus on Azure, Automation, DevOps, and Serverless. He works closely with clients to build solutions, mentor development teams and having fun during the whole process.
-In his spare time, he dives into the world of Bots, Machine Learning and 3D Graphics... then go on tropical holidays!</t>
+In his spare time, he is one of Australia's top Salsa teachers and is the 5 times Australian Salsa Champion and 5 times Australian Bachata Champion.</t>
   </si>
 </sst>
 </file>
@@ -984,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1027,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>8</v>
@@ -1055,13 +1070,13 @@
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>15</v>
@@ -1091,7 +1106,7 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
@@ -1124,15 +1139,17 @@
         <v>25</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1143,7 +1160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1163,13 +1180,13 @@
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="H5" s="3">
         <v>165</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>15</v>
@@ -1189,13 +1206,13 @@
         <v>30</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>32</v>
@@ -1237,13 +1254,13 @@
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H7" s="14">
         <v>245</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>21</v>
@@ -1257,7 +1274,7 @@
     </row>
     <row r="8" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>62</v>
@@ -1273,13 +1290,13 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
@@ -1316,7 +1333,9 @@
       <c r="H9" s="15">
         <v>245</v>
       </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="J9" s="15" t="s">
         <v>21</v>
       </c>
@@ -1347,7 +1366,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H10" s="3">
         <v>165</v>
@@ -1389,7 +1408,7 @@
         <v>245</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>21</v>
@@ -1427,7 +1446,7 @@
         <v>245</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>21</v>
@@ -1457,7 +1476,7 @@
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H13" s="3">
         <v>205</v>
@@ -1496,7 +1515,9 @@
       <c r="H14" s="3">
         <v>285</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="J14" s="3" t="s">
         <v>21</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>285</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>15</v>
@@ -1563,13 +1584,13 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="3" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="H16" s="3">
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>21</v>
@@ -1581,9 +1602,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
@@ -1599,7 +1620,7 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="H17" s="3">
         <v>245</v>
@@ -1615,31 +1636,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="3" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="H18" s="3">
         <v>50</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>21</v>
@@ -1651,9 +1672,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>35</v>
@@ -1668,16 +1689,16 @@
         <v>20</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>79</v>
+        <v>156</v>
       </c>
       <c r="H19" s="3">
         <v>245</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>21</v>
@@ -1689,9 +1710,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>62</v>
@@ -1706,16 +1727,16 @@
         <v>25</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>21</v>
@@ -1729,13 +1750,13 @@
     </row>
     <row r="21" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>13</v>
@@ -1744,16 +1765,16 @@
         <v>24</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H21" s="3">
         <v>285</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>15</v>
@@ -1767,7 +1788,7 @@
     </row>
     <row r="22" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
@@ -1779,19 +1800,19 @@
         <v>25</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>49</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>21</v>
@@ -1805,10 +1826,10 @@
     </row>
     <row r="23" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>38</v>
@@ -1817,13 +1838,13 @@
         <v>14</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H23" s="3">
         <v>225</v>
@@ -1841,10 +1862,10 @@
     </row>
     <row r="24" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>38</v>
@@ -1853,17 +1874,17 @@
         <v>14</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H24" s="3">
         <v>285</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
@@ -1875,28 +1896,30 @@
     </row>
     <row r="25" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H25" s="3">
         <v>245</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="J25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1909,7 +1932,7 @@
     </row>
     <row r="26" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -1925,7 +1948,7 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H26" s="3">
         <v>245</v>
@@ -1941,7 +1964,7 @@
     </row>
     <row r="27" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
@@ -1953,18 +1976,20 @@
         <v>18</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="J27" s="3" t="s">
         <v>15</v>
       </c>
@@ -1977,31 +2002,31 @@
     </row>
     <row r="28" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H28" s="3">
         <v>205</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>21</v>
@@ -2015,7 +2040,7 @@
     </row>
     <row r="29" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -2027,11 +2052,11 @@
         <v>18</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H29" s="3">
         <v>50</v>
@@ -2047,31 +2072,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H30" s="3">
         <v>225</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>15</v>
@@ -2085,31 +2110,31 @@
     </row>
     <row r="31" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H31" s="3">
         <v>285</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>21</v>
@@ -2133,21 +2158,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2305,10 +2315,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2330,19 +2365,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated seed data for superpowers tours
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\source\repos\ssw.consulting\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A0BFB6-F74B-4BF1-B274-88BB0D161A0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A65601-990A-4E4E-A3C4-F334DFC35167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="162">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Adam Cogan</t>
   </si>
   <si>
-    <t xml:space="preserve">Chief Architect, Microsoft Regional Director </t>
-  </si>
-  <si>
     <t>Azure DevOps</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Alex Breskin</t>
   </si>
   <si>
-    <t>Software Architect</t>
-  </si>
-  <si>
     <t>.NET Core</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Alvin Shen</t>
   </si>
   <si>
-    <t>China CEO</t>
-  </si>
-  <si>
     <t>Azure</t>
   </si>
   <si>
@@ -114,15 +105,9 @@
     <t>Andreas Lengkeek</t>
   </si>
   <si>
-    <t xml:space="preserve"> Senior Software Developer</t>
-  </si>
-  <si>
     <t>Andrew Forsyth</t>
   </si>
   <si>
-    <t>Video Producer/Director/Editor</t>
-  </si>
-  <si>
     <t>Office 365</t>
   </si>
   <si>
@@ -135,9 +120,6 @@
     <t>Anthony Ison</t>
   </si>
   <si>
-    <t>Senior Software Architect</t>
-  </si>
-  <si>
     <t>Planting roses</t>
   </si>
   <si>
@@ -204,9 +186,6 @@
     <t>Jason Taylor</t>
   </si>
   <si>
-    <t>Solution Architect</t>
-  </si>
-  <si>
     <t>Jason is a passionate, Solution Architect, trainer, mentor, and Full Stack Developer with 20 years professional experience. He works from our Brisbane office and currently specialises in building and teaching enterprise application development utilising .NET Core, Angular, Vue.js, and Azure. He's also a huge advocate for Clean Architecture and will also be presenting here at NDC.</t>
   </si>
   <si>
@@ -234,9 +213,6 @@
     <t>Ken Shi</t>
   </si>
   <si>
-    <t>User Experience Expert</t>
-  </si>
-  <si>
     <t>UX</t>
   </si>
   <si>
@@ -267,9 +243,6 @@
     <t>Matthew Sampias</t>
   </si>
   <si>
-    <t>State Manager - Queensland and International</t>
-  </si>
-  <si>
     <t>Power BI</t>
   </si>
   <si>
@@ -279,9 +252,6 @@
     <t>Michael Smedley</t>
   </si>
   <si>
-    <t>State Manager - Victoria</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
@@ -297,9 +267,6 @@
     <t>Penny Walker</t>
   </si>
   <si>
-    <t xml:space="preserve">Sales, Marketing and Onboarding Experience Guru </t>
-  </si>
-  <si>
     <t>Recruitment</t>
   </si>
   <si>
@@ -310,9 +277,6 @@
   </si>
   <si>
     <t>Ulysses Maclaren</t>
-  </si>
-  <si>
-    <t>General Manager</t>
   </si>
   <si>
     <t>Salsa</t>
@@ -499,6 +463,89 @@
   </si>
   <si>
     <t>Sebastien is a Software Architect with more than 10 years of experience in software development in France, China and now Australia. Before working for SSW, Sebastien worked for the world leading company for HR and Payroll, ADP, for 10 years, developing solutions used to pay hundreds of thousands employees.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSW Chief Architect, Microsoft Regional Director </t>
+  </si>
+  <si>
+    <t>SSW Software Architect</t>
+  </si>
+  <si>
+    <t>SSW China CEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SSW Senior Software Developer</t>
+  </si>
+  <si>
+    <t>SSW Video Producer/Director/Editor</t>
+  </si>
+  <si>
+    <t>SSW Senior Software Architect</t>
+  </si>
+  <si>
+    <t>SSW Solution Architect</t>
+  </si>
+  <si>
+    <t>SSW User Experience Expert</t>
+  </si>
+  <si>
+    <t>SSW State Manager - Queensland and International</t>
+  </si>
+  <si>
+    <t>SSW State Manager - Victoria</t>
+  </si>
+  <si>
+    <r>
+      <t>SSW</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Senior Software Architect</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SSW Sales, Marketing and Onboarding Experience Guru </t>
+  </si>
+  <si>
+    <t>SSW General Manager</t>
+  </si>
+  <si>
+    <t>Andrew Coates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft Senior Software Engineer </t>
+  </si>
+  <si>
+    <t>Andrew Coates is a Senior Software Engineer for Microsoft in Australia where he’s worked for over 15 years. His passions include teaching kids to code, learning &amp; using new technology and cricket (don’t ask him about it unless you want to talk about cricket for a LONG time).</t>
+  </si>
+  <si>
+    <t>@coatsy</t>
+  </si>
+  <si>
+    <t>Samantha Coates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BlitzBooks Author, Creator and Publisher</t>
+  </si>
+  <si>
+    <t>Samantha Coates is an internationally regarded pianist and presenter. She is the author, creator and publisher of BlitzBooks, the music education series that has brought laughter and creativity to music theory, sight reading and piano repertoire.</t>
   </si>
 </sst>
 </file>
@@ -536,7 +583,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -613,11 +660,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -663,6 +734,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,26 +1065,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="17.53515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
-    <col min="8" max="9" width="28.53515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.53515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.53515625" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="8.84375" style="2"/>
+    <col min="2" max="2" width="45.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.54296875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.36328125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="28.54296875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>8</v>
@@ -1035,998 +1123,1056 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="C4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="13" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="H5" s="3">
         <v>205</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3">
         <v>225</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H7" s="14">
         <v>245</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="J7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H9" s="15">
         <v>245</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="H10" s="3">
         <v>245</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H11" s="3">
         <v>245</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="H12" s="3">
         <v>205</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H13" s="3">
         <v>285</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>60</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H14" s="3">
         <v>285</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H15" s="3">
         <v>245</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="H16" s="3">
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H17" s="3">
         <v>205</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="J17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="E18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="F18" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H18" s="3">
         <v>245</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="H19" s="3">
         <v>285</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="F20" s="13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H21" s="3">
         <v>225</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H23" s="3">
         <v>285</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="H24" s="3">
         <v>245</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>90</v>
-      </c>
       <c r="G25" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H25" s="3">
         <v>205</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="H26" s="3">
         <v>205</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="116" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="102" x14ac:dyDescent="0.4">
-      <c r="A28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H28" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H28" s="14">
         <v>285</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>21</v>
+      <c r="I28" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="3">
+        <v>305</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" s="3">
+        <v>305</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2041,18 +2187,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2214,25 +2360,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix kosta spelling mistake
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\source\repos\ssw.consulting\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A65601-990A-4E4E-A3C4-F334DFC35167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EB9C2-12B8-4441-A2DE-C544F1B6FCCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Photoshop</t>
-  </si>
-  <si>
-    <t>Kosta Madorski</t>
   </si>
   <si>
     <t>Rock Climbing</t>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>Samantha Coates is an internationally regarded pianist and presenter. She is the author, creator and publisher of BlitzBooks, the music education series that has brought laughter and creativity to music theory, sight reading and piano repertoire.</t>
+  </si>
+  <si>
+    <t>Kosta Madorsky</t>
   </si>
 </sst>
 </file>
@@ -1067,25 +1067,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.54296875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="64.36328125" style="6" customWidth="1"/>
-    <col min="8" max="9" width="28.54296875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="2"/>
+    <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.23046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.53515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="28.53515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.53515625" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>8</v>
@@ -1123,12 +1123,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>12</v>
@@ -1139,13 +1139,13 @@
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="3">
         <v>305</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>14</v>
@@ -1157,12 +1157,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>16</v>
@@ -1175,13 +1175,13 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="3">
         <v>205</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>19</v>
@@ -1193,12 +1193,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>13</v>
@@ -1210,16 +1210,16 @@
         <v>22</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H4" s="3">
         <v>225</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>19</v>
@@ -1231,12 +1231,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="111.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>16</v>
@@ -1249,13 +1249,13 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="3">
         <v>205</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>14</v>
@@ -1267,21 +1267,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>26</v>
@@ -1293,7 +1293,7 @@
         <v>225</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>19</v>
@@ -1305,12 +1305,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>16</v>
@@ -1325,13 +1325,13 @@
         <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" s="14">
         <v>245</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>19</v>
@@ -1343,12 +1343,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>16</v>
@@ -1361,13 +1361,13 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" s="3">
         <v>245</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>19</v>
@@ -1379,12 +1379,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>31</v>
@@ -1405,7 +1405,7 @@
         <v>245</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>19</v>
@@ -1417,12 +1417,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>22</v>
@@ -1437,13 +1437,13 @@
         <v>39</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H10" s="3">
         <v>245</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>19</v>
@@ -1455,12 +1455,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>41</v>
@@ -1481,7 +1481,7 @@
         <v>245</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>19</v>
@@ -1493,12 +1493,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>47</v>
@@ -1511,13 +1511,13 @@
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="3">
         <v>205</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>19</v>
@@ -1529,12 +1529,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>16</v>
@@ -1553,7 +1553,7 @@
         <v>285</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>19</v>
@@ -1565,12 +1565,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>32</v>
@@ -1591,7 +1591,7 @@
         <v>285</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>14</v>
@@ -1603,12 +1603,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>16</v>
@@ -1621,13 +1621,13 @@
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H15" s="3">
         <v>245</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>19</v>
@@ -1639,12 +1639,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>16</v>
@@ -1657,13 +1657,13 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" s="3">
         <v>245</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>19</v>
@@ -1675,12 +1675,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>60</v>
@@ -1693,13 +1693,13 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" s="3">
         <v>205</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>19</v>
@@ -1711,12 +1711,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>16</v>
@@ -1728,16 +1728,16 @@
         <v>18</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H18" s="3">
         <v>245</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>19</v>
@@ -1749,12 +1749,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>16</v>
@@ -1766,16 +1766,16 @@
         <v>22</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H19" s="3">
         <v>285</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>19</v>
@@ -1787,15 +1787,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>12</v>
@@ -1804,16 +1804,16 @@
         <v>21</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="H20" s="3">
         <v>285</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>14</v>
@@ -1825,12 +1825,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>16</v>
@@ -1839,19 +1839,19 @@
         <v>22</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H21" s="3">
         <v>225</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>19</v>
@@ -1863,12 +1863,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>31</v>
@@ -1877,19 +1877,19 @@
         <v>13</v>
       </c>
       <c r="E22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>19</v>
@@ -1901,12 +1901,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>31</v>
@@ -1915,17 +1915,17 @@
         <v>13</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H23" s="3">
         <v>285</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
@@ -1935,12 +1935,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="83" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="83.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>16</v>
@@ -1953,13 +1953,13 @@
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="3">
         <v>245</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
@@ -1969,33 +1969,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="66.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H25" s="3">
         <v>205</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>19</v>
@@ -2007,12 +2007,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>18</v>
@@ -2021,17 +2021,17 @@
         <v>16</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H26" s="3">
         <v>205</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>19</v>
@@ -2043,31 +2043,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H27" s="3">
         <v>225</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>14</v>
@@ -2079,33 +2079,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="17" t="s">
+      <c r="D28" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="E28" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="F28" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="18" t="s">
-        <v>87</v>
-      </c>
       <c r="G28" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H28" s="14">
         <v>285</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>19</v>
@@ -2117,49 +2117,49 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="45.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="3">
         <v>305</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="48.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="J29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="B30" s="19" t="s">
         <v>159</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>160</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H30" s="3">
         <v>305</v>
@@ -2187,21 +2187,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2359,31 +2344,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2399,4 +2375,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated seed data to indicate ssw staff
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Source\Repos\SSWConsulting\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EB9C2-12B8-4441-A2DE-C544F1B6FCCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E176C8-9786-476C-824F-7735A4AA86FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$28</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>Kosta Madorsky</t>
+  </si>
+  <si>
+    <t>IsExternal?</t>
   </si>
 </sst>
 </file>
@@ -1065,27 +1068,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.23046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.53515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
-    <col min="8" max="9" width="28.53515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.53515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.53515625" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="8.84375" style="2"/>
+    <col min="2" max="2" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" style="6" customWidth="1"/>
+    <col min="8" max="10" width="28.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1114,16 +1117,19 @@
         <v>94</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1147,8 +1153,8 @@
       <c r="I2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
+      <c r="J2" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>14</v>
@@ -1156,8 +1162,11 @@
       <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1183,8 +1192,8 @@
       <c r="I3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
+      <c r="J3" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>19</v>
@@ -1192,8 +1201,11 @@
       <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="M3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1221,8 +1233,8 @@
       <c r="I4" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>19</v>
+      <c r="J4" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>19</v>
@@ -1230,8 +1242,11 @@
       <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="111.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="4" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1257,8 +1272,8 @@
       <c r="I5" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>14</v>
+      <c r="J5" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>14</v>
@@ -1266,8 +1281,11 @@
       <c r="L5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="M5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1295,17 +1313,20 @@
       <c r="I6" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>19</v>
+      <c r="J6" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="M6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1333,17 +1354,20 @@
       <c r="I7" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="14" t="s">
-        <v>19</v>
+      <c r="J7" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M7" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1369,8 +1393,8 @@
       <c r="I8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>19</v>
+      <c r="J8" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>19</v>
@@ -1378,8 +1402,11 @@
       <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1407,17 +1434,20 @@
       <c r="I9" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="15" t="s">
-        <v>19</v>
+      <c r="J9" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="M9" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1445,17 +1475,20 @@
       <c r="I10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>19</v>
+      <c r="J10" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1483,17 +1516,20 @@
       <c r="I11" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>19</v>
+      <c r="J11" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1519,8 +1555,8 @@
       <c r="I12" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>19</v>
+      <c r="J12" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>19</v>
@@ -1528,8 +1564,11 @@
       <c r="L12" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1555,17 +1594,20 @@
       <c r="I13" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>19</v>
+      <c r="J13" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1593,8 +1635,8 @@
       <c r="I14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>14</v>
+      <c r="J14" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>14</v>
@@ -1602,8 +1644,11 @@
       <c r="L14" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="M14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1629,17 +1674,20 @@
       <c r="I15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>19</v>
+      <c r="J15" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="M15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1665,17 +1713,20 @@
       <c r="I16" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>19</v>
+      <c r="J16" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1701,17 +1752,20 @@
       <c r="I17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>19</v>
+      <c r="J17" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>161</v>
       </c>
@@ -1739,8 +1793,8 @@
       <c r="I18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>19</v>
+      <c r="J18" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>19</v>
@@ -1748,8 +1802,11 @@
       <c r="L18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="M18" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -1777,17 +1834,20 @@
       <c r="I19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>19</v>
+      <c r="J19" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1815,8 +1875,8 @@
       <c r="I20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>14</v>
+      <c r="J20" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>14</v>
@@ -1824,8 +1884,11 @@
       <c r="L20" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+      <c r="M20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -1853,17 +1916,20 @@
       <c r="I21" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>19</v>
+      <c r="J21" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1891,17 +1957,20 @@
       <c r="I22" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>19</v>
+      <c r="J22" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -1927,15 +1996,18 @@
       <c r="I23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="J23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="83.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -1961,15 +2033,18 @@
       <c r="I24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="J24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="66.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -1997,8 +2072,8 @@
       <c r="I25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>19</v>
+      <c r="J25" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>19</v>
@@ -2006,8 +2081,11 @@
       <c r="L25" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="M25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -2033,8 +2111,8 @@
       <c r="I26" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>19</v>
+      <c r="J26" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>19</v>
@@ -2042,8 +2120,11 @@
       <c r="L26" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+      <c r="M26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -2069,17 +2150,20 @@
       <c r="I27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>14</v>
+      <c r="J27" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="102" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>82</v>
       </c>
@@ -2107,8 +2191,8 @@
       <c r="I28" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>19</v>
+      <c r="J28" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>19</v>
@@ -2116,8 +2200,11 @@
       <c r="L28" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="45.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M28" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>154</v>
       </c>
@@ -2137,17 +2224,20 @@
       <c r="I29" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J29" s="3" t="s">
-        <v>19</v>
+      <c r="J29" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="48.55" customHeight="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>158</v>
       </c>
@@ -2165,19 +2255,22 @@
         <v>305</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="3" t="s">
+      <c r="J30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L28" xr:uid="{9AA24026-1D6B-4950-9702-5DBD73A8EC72}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
+  <autoFilter ref="A1:M28" xr:uid="{9AA24026-1D6B-4950-9702-5DBD73A8EC72}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M28">
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
@@ -2388,15 +2481,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add christian, paris and ug event
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Source\Repos\SSWConsulting\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E176C8-9786-476C-824F-7735A4AA86FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3561D50-9E49-4B09-A116-7861E2CEFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="168">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -549,6 +549,23 @@
   </si>
   <si>
     <t>IsExternal?</t>
+  </si>
+  <si>
+    <t>Paris Lowres</t>
+  </si>
+  <si>
+    <t>SSW Office Assistant</t>
+  </si>
+  <si>
+    <t>Christian Morford-Waite</t>
+  </si>
+  <si>
+    <t>Paris is a copy editor at university and working for SSW while finishing her degree. Paris makes the Melbourne office run smoothly!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">​​​​​​​​​​Christian is a Software Developer with over 5 years of experience working with a wide range of technologies and Azure resources.
+Specialising in backend .NET development and API integration. He enjoys working on process improvement and automation through PowerShell scripting and Azure Build Pipelines.
+</t>
   </si>
 </sst>
 </file>
@@ -1068,27 +1085,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="64.42578125" style="6" customWidth="1"/>
-    <col min="8" max="10" width="28.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.53515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
+    <col min="8" max="10" width="28.53515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.53515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.53515625" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1205,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="4" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,7 +1302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1367,7 +1384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1406,7 +1423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1488,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1529,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1568,7 +1585,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1607,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1648,7 +1665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1687,7 +1704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>161</v>
       </c>
@@ -1806,7 +1823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -1847,7 +1864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1888,7 +1905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -1929,7 +1946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1970,7 +1987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -2007,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="83.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -2044,7 +2061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -2085,7 +2102,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -2124,7 +2141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -2163,7 +2180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
         <v>82</v>
       </c>
@@ -2204,7 +2221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="45.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="19" t="s">
         <v>154</v>
       </c>
@@ -2237,7 +2254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19" t="s">
         <v>158</v>
       </c>
@@ -2265,6 +2282,82 @@
         <v>14</v>
       </c>
       <c r="M30" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="3">
+        <v>205</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H32" s="3">
+        <v>205</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2280,6 +2373,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2437,22 +2545,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2468,28 +2585,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add christian, paris and ug event (#65)
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Source\Repos\SSWConsulting\SSW.Consulting\SeedData\profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E176C8-9786-476C-824F-7735A4AA86FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3561D50-9E49-4B09-A116-7861E2CEFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="168">
   <si>
     <t>Employee Profile</t>
   </si>
@@ -549,6 +549,23 @@
   </si>
   <si>
     <t>IsExternal?</t>
+  </si>
+  <si>
+    <t>Paris Lowres</t>
+  </si>
+  <si>
+    <t>SSW Office Assistant</t>
+  </si>
+  <si>
+    <t>Christian Morford-Waite</t>
+  </si>
+  <si>
+    <t>Paris is a copy editor at university and working for SSW while finishing her degree. Paris makes the Melbourne office run smoothly!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">​​​​​​​​​​Christian is a Software Developer with over 5 years of experience working with a wide range of technologies and Azure resources.
+Specialising in backend .NET development and API integration. He enjoys working on process improvement and automation through PowerShell scripting and Azure Build Pipelines.
+</t>
   </si>
 </sst>
 </file>
@@ -1068,27 +1085,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="64.42578125" style="6" customWidth="1"/>
-    <col min="8" max="10" width="28.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="45.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.53515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="64.3828125" style="6" customWidth="1"/>
+    <col min="8" max="10" width="28.53515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.53515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.53515625" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1205,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="4" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,7 +1302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1367,7 +1384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1406,7 +1423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1488,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1529,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1568,7 +1585,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1607,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1648,7 +1665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1687,7 +1704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>161</v>
       </c>
@@ -1806,7 +1823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -1847,7 +1864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1888,7 +1905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -1929,7 +1946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1970,7 +1987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -2007,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="83.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -2044,7 +2061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -2085,7 +2102,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -2124,7 +2141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -2163,7 +2180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
         <v>82</v>
       </c>
@@ -2204,7 +2221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="45.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="19" t="s">
         <v>154</v>
       </c>
@@ -2237,7 +2254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19" t="s">
         <v>158</v>
       </c>
@@ -2265,6 +2282,82 @@
         <v>14</v>
       </c>
       <c r="M30" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="3">
+        <v>205</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H32" s="3">
+        <v>205</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2280,6 +2373,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2437,22 +2545,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2468,28 +2585,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update guest flag for paris and christian
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3561D50-9E49-4B09-A116-7861E2CEFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23154EE7-5040-45B8-853A-5185E65A2E5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2310,7 +2310,7 @@
         <v>132</v>
       </c>
       <c r="J31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>19</v>
@@ -2349,7 +2349,7 @@
         <v>132</v>
       </c>
       <c r="J32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>19</v>
@@ -2373,21 +2373,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2545,31 +2530,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2585,4 +2561,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update guest flag for paris and christian (#66)
</commit_message>
<xml_diff>
--- a/SeedData/profiles/NDC-Profiles-2019.xlsx
+++ b/SeedData/profiles/NDC-Profiles-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\SSW.Consulting\SeedData\profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3561D50-9E49-4B09-A116-7861E2CEFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23154EE7-5040-45B8-853A-5185E65A2E5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2310,7 +2310,7 @@
         <v>132</v>
       </c>
       <c r="J31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>19</v>
@@ -2349,7 +2349,7 @@
         <v>132</v>
       </c>
       <c r="J32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>19</v>
@@ -2373,21 +2373,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034E37261CDFF6E499617785CBCCDDF16" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95605b472c394c37ef9b7182a30493b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2501a265-b72f-461c-b9b9-7718c9bea790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34d3549c5192401b359f168ea9918421" ns2:_="">
     <xsd:import namespace="2501a265-b72f-461c-b9b9-7718c9bea790"/>
@@ -2545,31 +2530,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97CB9D17-4477-4DF4-8809-23EB0015B94F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2585,4 +2561,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8019B69C-5AB0-4D90-A022-C89624733A67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F375BB27-CB7A-4327-84D4-34D442AD2CE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2501a265-b72f-461c-b9b9-7718c9bea790"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>